<commit_message>
serial numbers added 2
</commit_message>
<xml_diff>
--- a/Paper I.xlsx
+++ b/Paper I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C560DBB4-B176-4B6E-BFA1-9299018E37FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC123F0-FF77-4026-89A2-C027BE861141}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Regional</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>BASIC ENGLISH</t>
+  </si>
+  <si>
+    <t>Telanagana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India </t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -288,17 +297,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,8 +321,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,11 +619,12 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="60.42578125" customWidth="1"/>
     <col min="5" max="10" width="45.7109375" customWidth="1"/>
   </cols>
@@ -616,35 +638,41 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A3" s="12"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" s="11" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
@@ -652,7 +680,7 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
@@ -660,7 +688,7 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="2"/>
@@ -668,7 +696,7 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="2"/>
@@ -676,7 +704,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="2"/>
@@ -684,7 +712,7 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="2"/>
@@ -692,7 +720,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" s="2"/>
@@ -700,7 +728,7 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
       <c r="B12" s="2"/>
@@ -708,7 +736,7 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="2"/>
@@ -716,7 +744,7 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
       <c r="B14" s="2"/>
@@ -724,7 +752,7 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="3">
         <v>12</v>
       </c>
       <c r="B15" s="2"/>
@@ -732,7 +760,7 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
       <c r="B16" s="2"/>
@@ -757,11 +785,12 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="160.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -772,81 +801,115 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
   </sheetData>
@@ -865,11 +928,12 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="160.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -880,81 +944,115 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
   </sheetData>
@@ -977,6 +1075,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="59" customWidth="1"/>
   </cols>
   <sheetData>
@@ -989,10 +1088,10 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1003,109 +1102,143 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1126,12 +1259,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378D551E-1EFA-42D7-ADEC-518327CDCC9F}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="160.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1142,81 +1276,115 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
   </sheetData>
@@ -1234,12 +1402,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="84.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1251,103 +1419,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1367,11 +1569,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="86" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1383,103 +1586,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1499,11 +1736,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="86" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1515,103 +1753,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1631,11 +1903,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="86" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1647,103 +1920,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1763,11 +2070,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="86" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1779,103 +2087,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1895,11 +2237,12 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="86" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1911,103 +2254,137 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -2026,12 +2403,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EE5766-CF84-455F-8C74-FDA420927216}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2046,10 +2424,10 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2061,20 +2439,22 @@
       <c r="E2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2082,7 +2462,9 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -2090,7 +2472,9 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2098,7 +2482,9 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2106,7 +2492,9 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2114,7 +2502,9 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2122,7 +2512,9 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2130,7 +2522,9 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2138,7 +2532,9 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2146,7 +2542,9 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2154,7 +2552,9 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2162,7 +2562,9 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2170,7 +2572,9 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2178,7 +2582,9 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2186,7 +2592,9 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2194,7 +2602,9 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2202,7 +2612,9 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2233,6 +2645,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="153.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2243,83 +2656,117 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
   </sheetData>

</xml_diff>